<commit_message>
Deactivate interpolation of spike removal
</commit_message>
<xml_diff>
--- a/Resources/EmpreinteVariableDescription.xlsx
+++ b/Resources/EmpreinteVariableDescription.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Berge" sheetId="1" r:id="rId1"/>
@@ -13,8 +13,9 @@
     <sheet name="Foret_neige" sheetId="7" r:id="rId4"/>
     <sheet name="Foret_sol" sheetId="3" r:id="rId5"/>
     <sheet name="Reservoir" sheetId="2" r:id="rId6"/>
-    <sheet name="Thermistors" sheetId="8" r:id="rId7"/>
-    <sheet name="Notations and abbreviations" sheetId="4" r:id="rId8"/>
+    <sheet name="Riviere" sheetId="9" r:id="rId7"/>
+    <sheet name="Thermistors" sheetId="8" r:id="rId8"/>
+    <sheet name="Notations and abbreviations" sheetId="4" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2466" uniqueCount="1051">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2668" uniqueCount="1086">
   <si>
     <t>LI-7700</t>
   </si>
@@ -3179,6 +3180,111 @@
   </si>
   <si>
     <t>pumpOn_LI7700</t>
+  </si>
+  <si>
+    <t>Acquisition frequency: 1 min</t>
+  </si>
+  <si>
+    <t>BattV_Min</t>
+  </si>
+  <si>
+    <t>PTemp_C_Avg</t>
+  </si>
+  <si>
+    <t>CNR4TC_Avg</t>
+  </si>
+  <si>
+    <t>RsNet_Avg</t>
+  </si>
+  <si>
+    <t>RlNet_Avg</t>
+  </si>
+  <si>
+    <t>AirTC_Avg</t>
+  </si>
+  <si>
+    <t>AirTC_Min</t>
+  </si>
+  <si>
+    <t>AirTC_Max</t>
+  </si>
+  <si>
+    <t>WS_ms_Avg</t>
+  </si>
+  <si>
+    <t>WS_ms_S_WVT</t>
+  </si>
+  <si>
+    <t>WindDir_D1_WVT</t>
+  </si>
+  <si>
+    <t>WindDir_SD1_WVT</t>
+  </si>
+  <si>
+    <t>T107_C_Avg</t>
+  </si>
+  <si>
+    <t>T107_C_Min</t>
+  </si>
+  <si>
+    <t>T107_C_Max</t>
+  </si>
+  <si>
+    <t>Rain_mm_Tot</t>
+  </si>
+  <si>
+    <t>BattV</t>
+  </si>
+  <si>
+    <t>PTemp_C</t>
+  </si>
+  <si>
+    <t>Long wave net radiation</t>
+  </si>
+  <si>
+    <t>Short wave net radiation</t>
+  </si>
+  <si>
+    <t>CR5000</t>
+  </si>
+  <si>
+    <t>Minimum water temperature</t>
+  </si>
+  <si>
+    <t>Maximum water temperature</t>
+  </si>
+  <si>
+    <t>precip_TB3</t>
+  </si>
+  <si>
+    <t>TB3</t>
+  </si>
+  <si>
+    <t>water_temp_avg_T107C</t>
+  </si>
+  <si>
+    <t>water_temp_min_T107C</t>
+  </si>
+  <si>
+    <t>water_temp_max_T107C</t>
+  </si>
+  <si>
+    <t>T107C</t>
+  </si>
+  <si>
+    <t>Thermistor</t>
+  </si>
+  <si>
+    <t>CNR4: 2 m</t>
+  </si>
+  <si>
+    <t>HMP45C: 2 m</t>
+  </si>
+  <si>
+    <t>TB3: 1 m</t>
+  </si>
+  <si>
+    <t>05103: 2 m</t>
   </si>
 </sst>
 </file>
@@ -3624,8 +3730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G381"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView topLeftCell="B30" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -45566,6 +45672,737 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="62.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="B1" s="23" t="s">
+        <v>647</v>
+      </c>
+      <c r="E1" s="18"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B2" s="5" t="s">
+        <v>644</v>
+      </c>
+      <c r="E2" s="18"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="5" t="s">
+        <v>645</v>
+      </c>
+      <c r="E3" s="18"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="5" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E4" s="18"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="5" t="s">
+        <v>656</v>
+      </c>
+      <c r="E5" s="18"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="21" t="s">
+        <v>1082</v>
+      </c>
+      <c r="E6" s="18"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="21" t="s">
+        <v>1083</v>
+      </c>
+      <c r="E7" s="18"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="21" t="s">
+        <v>1084</v>
+      </c>
+      <c r="E8" s="18"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="21" t="s">
+        <v>1085</v>
+      </c>
+      <c r="E9" s="18"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="5"/>
+      <c r="E10" s="18"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E12" s="18"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>397</v>
+      </c>
+      <c r="B13" t="s">
+        <v>189</v>
+      </c>
+      <c r="C13" t="s">
+        <v>202</v>
+      </c>
+      <c r="D13" t="s">
+        <v>203</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>1072</v>
+      </c>
+      <c r="F13" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>453</v>
+      </c>
+      <c r="B14" t="s">
+        <v>739</v>
+      </c>
+      <c r="C14" t="s">
+        <v>457</v>
+      </c>
+      <c r="D14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>460</v>
+      </c>
+      <c r="F14" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>945</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>1054</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>554</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>454</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1057</v>
+      </c>
+      <c r="C16" t="s">
+        <v>208</v>
+      </c>
+      <c r="D16" t="s">
+        <v>142</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>460</v>
+      </c>
+      <c r="F16" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>456</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1058</v>
+      </c>
+      <c r="C17" t="s">
+        <v>208</v>
+      </c>
+      <c r="D17" t="s">
+        <v>142</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>460</v>
+      </c>
+      <c r="F17" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>455</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1059</v>
+      </c>
+      <c r="C18" t="s">
+        <v>208</v>
+      </c>
+      <c r="D18" t="s">
+        <v>142</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>460</v>
+      </c>
+      <c r="F18" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>408</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1052</v>
+      </c>
+      <c r="C19" t="s">
+        <v>394</v>
+      </c>
+      <c r="D19" t="s">
+        <v>117</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>1072</v>
+      </c>
+      <c r="F19" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>408</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1068</v>
+      </c>
+      <c r="C20" t="s">
+        <v>394</v>
+      </c>
+      <c r="D20" t="s">
+        <v>117</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>1072</v>
+      </c>
+      <c r="F20" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C21" t="s">
+        <v>512</v>
+      </c>
+      <c r="D21" t="s">
+        <v>364</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>1076</v>
+      </c>
+      <c r="F21" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>938</v>
+      </c>
+      <c r="B22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" t="s">
+        <v>516</v>
+      </c>
+      <c r="D22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="F22" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>939</v>
+      </c>
+      <c r="B23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" t="s">
+        <v>517</v>
+      </c>
+      <c r="D23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="F23" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="B24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>520</v>
+      </c>
+      <c r="D24" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="F24" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>940</v>
+      </c>
+      <c r="B25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" t="s">
+        <v>521</v>
+      </c>
+      <c r="D25" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="F25" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>955</v>
+      </c>
+      <c r="B26" t="s">
+        <v>366</v>
+      </c>
+      <c r="C26" t="s">
+        <v>550</v>
+      </c>
+      <c r="D26" t="s">
+        <v>534</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>551</v>
+      </c>
+      <c r="F26" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>955</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1062</v>
+      </c>
+      <c r="C27" t="s">
+        <v>550</v>
+      </c>
+      <c r="D27" t="s">
+        <v>534</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>551</v>
+      </c>
+      <c r="F27" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>956</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1060</v>
+      </c>
+      <c r="C28" t="s">
+        <v>552</v>
+      </c>
+      <c r="D28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>551</v>
+      </c>
+      <c r="F28" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>956</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1061</v>
+      </c>
+      <c r="C29" t="s">
+        <v>552</v>
+      </c>
+      <c r="D29" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>551</v>
+      </c>
+      <c r="F29" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>1077</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1064</v>
+      </c>
+      <c r="C30" t="s">
+        <v>678</v>
+      </c>
+      <c r="D30" t="s">
+        <v>142</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>1080</v>
+      </c>
+      <c r="F30" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>1078</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1065</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1073</v>
+      </c>
+      <c r="D31" t="s">
+        <v>142</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>1080</v>
+      </c>
+      <c r="F31" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>1079</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1074</v>
+      </c>
+      <c r="D32" t="s">
+        <v>142</v>
+      </c>
+      <c r="E32" s="18" t="s">
+        <v>1080</v>
+      </c>
+      <c r="F32" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>226</v>
+      </c>
+      <c r="B33" t="s">
+        <v>190</v>
+      </c>
+      <c r="C33" t="s">
+        <v>204</v>
+      </c>
+      <c r="D33" t="s">
+        <v>203</v>
+      </c>
+      <c r="E33" s="18" t="s">
+        <v>1072</v>
+      </c>
+      <c r="F33" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>226</v>
+      </c>
+      <c r="B34" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" t="s">
+        <v>126</v>
+      </c>
+      <c r="D34" t="s">
+        <v>203</v>
+      </c>
+      <c r="E34" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="F34" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>226</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1055</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1071</v>
+      </c>
+      <c r="D35" t="s">
+        <v>39</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="F35" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>226</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1056</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1070</v>
+      </c>
+      <c r="D36" t="s">
+        <v>39</v>
+      </c>
+      <c r="E36" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="F36" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>226</v>
+      </c>
+      <c r="B37" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37" t="s">
+        <v>558</v>
+      </c>
+      <c r="D37" t="s">
+        <v>39</v>
+      </c>
+      <c r="E37" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="F37" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>226</v>
+      </c>
+      <c r="B38" t="s">
+        <v>41</v>
+      </c>
+      <c r="C38" t="s">
+        <v>517</v>
+      </c>
+      <c r="D38" t="s">
+        <v>39</v>
+      </c>
+      <c r="E38" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="F38" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>226</v>
+      </c>
+      <c r="B39" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" t="s">
+        <v>516</v>
+      </c>
+      <c r="D39" t="s">
+        <v>39</v>
+      </c>
+      <c r="E39" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="F39" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>226</v>
+      </c>
+      <c r="B40" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C40" t="s">
+        <v>509</v>
+      </c>
+      <c r="D40" t="s">
+        <v>142</v>
+      </c>
+      <c r="E40" s="18" t="s">
+        <v>1072</v>
+      </c>
+      <c r="F40" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>226</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1069</v>
+      </c>
+      <c r="C41" t="s">
+        <v>509</v>
+      </c>
+      <c r="D41" t="s">
+        <v>142</v>
+      </c>
+      <c r="E41" s="18" t="s">
+        <v>1072</v>
+      </c>
+      <c r="F41" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>554</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E42" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>226</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1063</v>
+      </c>
+      <c r="C43" t="s">
+        <v>550</v>
+      </c>
+      <c r="D43" t="s">
+        <v>534</v>
+      </c>
+      <c r="E43" s="18" t="s">
+        <v>551</v>
+      </c>
+      <c r="F43" t="s">
+        <v>537</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="E26 E27:E29 E43" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -45695,7 +46532,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>

</xml_diff>

<commit_message>
Temporarily solve reindex issue
</commit_message>
<xml_diff>
--- a/Resources/EmpreinteVariableDescription.xlsx
+++ b/Resources/EmpreinteVariableDescription.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Berge" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2668" uniqueCount="1086">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2668" uniqueCount="1104">
   <si>
     <t>LI-7700</t>
   </si>
@@ -2963,15 +2963,6 @@
     <t>CH4_strg</t>
   </si>
   <si>
-    <t>qc_CO2_flux</t>
-  </si>
-  <si>
-    <t>rand_err_CO2_flux</t>
-  </si>
-  <si>
-    <t>CO2_v-adv</t>
-  </si>
-  <si>
     <t>CO2_molar_density</t>
   </si>
   <si>
@@ -2981,36 +2972,9 @@
     <t>CO2_mixing_ratio</t>
   </si>
   <si>
-    <t>CO2_time_lag</t>
-  </si>
-  <si>
-    <t>CO2_def_timelag</t>
-  </si>
-  <si>
-    <t>un_CO2_flux</t>
-  </si>
-  <si>
-    <t>CO2_scf</t>
-  </si>
-  <si>
     <t>CO2_spikes</t>
   </si>
   <si>
-    <t>CO2_var</t>
-  </si>
-  <si>
-    <t>w/CO2_cov</t>
-  </si>
-  <si>
-    <t>qc_H2O_flux</t>
-  </si>
-  <si>
-    <t>rand_err_H2O_flux</t>
-  </si>
-  <si>
-    <t>H2O_v-adv</t>
-  </si>
-  <si>
     <t>H2O_molar_density</t>
   </si>
   <si>
@@ -3020,36 +2984,9 @@
     <t>H2O_mixing_ratio</t>
   </si>
   <si>
-    <t>H2O_time_lag</t>
-  </si>
-  <si>
-    <t>H2O_def_timelag</t>
-  </si>
-  <si>
-    <t>un_H2O_flux</t>
-  </si>
-  <si>
-    <t>H2O_scf</t>
-  </si>
-  <si>
     <t>H2O_spikes</t>
   </si>
   <si>
-    <t>H2O_var</t>
-  </si>
-  <si>
-    <t>w/H2O_cov</t>
-  </si>
-  <si>
-    <t>qc_CH4_flux</t>
-  </si>
-  <si>
-    <t>rand_err_CH4_flux</t>
-  </si>
-  <si>
-    <t>CH4_v-adv</t>
-  </si>
-  <si>
     <t>CH4_molar_density</t>
   </si>
   <si>
@@ -3059,18 +2996,6 @@
     <t>CH4_mixing_ratio</t>
   </si>
   <si>
-    <t>CH4_time_lag</t>
-  </si>
-  <si>
-    <t>CH4_def_timelag</t>
-  </si>
-  <si>
-    <t>un_CH4_flux</t>
-  </si>
-  <si>
-    <t>CH4_scf</t>
-  </si>
-  <si>
     <t>8u/v/w/ts/CO2/H2O/CH4/none</t>
   </si>
   <si>
@@ -3080,12 +3005,6 @@
     <t>CH4_spikes</t>
   </si>
   <si>
-    <t>CH4_var</t>
-  </si>
-  <si>
-    <t>w/CH4_cov</t>
-  </si>
-  <si>
     <t>air_temp</t>
   </si>
   <si>
@@ -3285,6 +3204,141 @@
   </si>
   <si>
     <t>05103: 2 m</t>
+  </si>
+  <si>
+    <t>qc_ch4_flux</t>
+  </si>
+  <si>
+    <t>ch4_flux</t>
+  </si>
+  <si>
+    <t>rand_err_ch4_flux</t>
+  </si>
+  <si>
+    <t>ch4_mixing_ratio</t>
+  </si>
+  <si>
+    <t>ch4_molar_density</t>
+  </si>
+  <si>
+    <t>ch4_mole_fraction</t>
+  </si>
+  <si>
+    <t>ch4_spikes</t>
+  </si>
+  <si>
+    <t>ch4_strg</t>
+  </si>
+  <si>
+    <t>ch4_v-adv</t>
+  </si>
+  <si>
+    <t>ch4_time_lag</t>
+  </si>
+  <si>
+    <t>ch4_def_timelag</t>
+  </si>
+  <si>
+    <t>un_ch4_flux</t>
+  </si>
+  <si>
+    <t>ch4_scf</t>
+  </si>
+  <si>
+    <t>ch4_var</t>
+  </si>
+  <si>
+    <t>w/ch4_cov</t>
+  </si>
+  <si>
+    <t>co2_flux</t>
+  </si>
+  <si>
+    <t>qc_co2_flux</t>
+  </si>
+  <si>
+    <t>rand_err_co2_flux</t>
+  </si>
+  <si>
+    <t>co2_mixing_ratio</t>
+  </si>
+  <si>
+    <t>co2_molar_density</t>
+  </si>
+  <si>
+    <t>co2_mole_fraction</t>
+  </si>
+  <si>
+    <t>co2_spikes</t>
+  </si>
+  <si>
+    <t>co2_strg</t>
+  </si>
+  <si>
+    <t>co2_v-adv</t>
+  </si>
+  <si>
+    <t>co2_time_lag</t>
+  </si>
+  <si>
+    <t>co2_def_timelag</t>
+  </si>
+  <si>
+    <t>un_co2_flux</t>
+  </si>
+  <si>
+    <t>co2_scf</t>
+  </si>
+  <si>
+    <t>co2_var</t>
+  </si>
+  <si>
+    <t>w/co2_cov</t>
+  </si>
+  <si>
+    <t>h2o_flux</t>
+  </si>
+  <si>
+    <t>qc_h2o_flux</t>
+  </si>
+  <si>
+    <t>rand_err_h2o_flux</t>
+  </si>
+  <si>
+    <t>h2o_mixing_ratio</t>
+  </si>
+  <si>
+    <t>h2o_molar_density</t>
+  </si>
+  <si>
+    <t>h2o_mole_fraction</t>
+  </si>
+  <si>
+    <t>h2o_spikes</t>
+  </si>
+  <si>
+    <t>h2o_strg</t>
+  </si>
+  <si>
+    <t>h2o_v-adv</t>
+  </si>
+  <si>
+    <t>h2o_time_lag</t>
+  </si>
+  <si>
+    <t>h2o_def_timelag</t>
+  </si>
+  <si>
+    <t>un_h2o_flux</t>
+  </si>
+  <si>
+    <t>h2o_scf</t>
+  </si>
+  <si>
+    <t>h2o_var</t>
+  </si>
+  <si>
+    <t>w/h2o_cov</t>
   </si>
 </sst>
 </file>
@@ -3730,8 +3784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G381"/>
   <sheetViews>
-    <sheetView topLeftCell="B30" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7316,7 +7370,7 @@
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>1020</v>
+        <v>993</v>
       </c>
       <c r="B207" t="s">
         <v>725</v>
@@ -7330,7 +7384,7 @@
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A208" s="31" t="s">
-        <v>1047</v>
+        <v>1020</v>
       </c>
       <c r="B208" t="s">
         <v>739</v>
@@ -7344,7 +7398,7 @@
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A209" s="31" t="s">
-        <v>1046</v>
+        <v>1019</v>
       </c>
       <c r="B209" t="s">
         <v>737</v>
@@ -7358,7 +7412,7 @@
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>1019</v>
+        <v>992</v>
       </c>
       <c r="B210" t="s">
         <v>724</v>
@@ -7372,7 +7426,7 @@
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A211" s="31" t="s">
-        <v>1048</v>
+        <v>1021</v>
       </c>
       <c r="B211" t="s">
         <v>741</v>
@@ -7386,7 +7440,7 @@
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>1032</v>
+        <v>1005</v>
       </c>
       <c r="B212" t="s">
         <v>794</v>
@@ -7397,7 +7451,7 @@
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A213" s="31" t="s">
-        <v>1045</v>
+        <v>1018</v>
       </c>
       <c r="B213" t="s">
         <v>80</v>
@@ -7434,7 +7488,7 @@
         <v>173</v>
       </c>
       <c r="B215" t="s">
-        <v>173</v>
+        <v>1060</v>
       </c>
       <c r="C215" t="s">
         <v>856</v>
@@ -7448,7 +7502,7 @@
         <v>973</v>
       </c>
       <c r="B216" t="s">
-        <v>1004</v>
+        <v>1059</v>
       </c>
       <c r="C216" t="s">
         <v>859</v>
@@ -7466,7 +7520,7 @@
         <v>974</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>1005</v>
+        <v>1061</v>
       </c>
       <c r="C217" s="3" t="s">
         <v>867</v>
@@ -7480,10 +7534,10 @@
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>1009</v>
+        <v>988</v>
       </c>
       <c r="B218" t="s">
-        <v>1009</v>
+        <v>1062</v>
       </c>
       <c r="C218" t="s">
         <v>888</v>
@@ -7494,10 +7548,10 @@
     </row>
     <row r="219" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>1007</v>
+        <v>986</v>
       </c>
       <c r="B219" t="s">
-        <v>1007</v>
+        <v>1063</v>
       </c>
       <c r="C219" t="s">
         <v>886</v>
@@ -7512,10 +7566,10 @@
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>1008</v>
+        <v>987</v>
       </c>
       <c r="B220" t="s">
-        <v>1008</v>
+        <v>1064</v>
       </c>
       <c r="C220" t="s">
         <v>887</v>
@@ -7529,10 +7583,10 @@
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>1016</v>
+        <v>991</v>
       </c>
       <c r="B221" t="s">
-        <v>1016</v>
+        <v>1065</v>
       </c>
       <c r="D221" t="s">
         <v>693</v>
@@ -7543,7 +7597,7 @@
         <v>977</v>
       </c>
       <c r="B222" t="s">
-        <v>977</v>
+        <v>1066</v>
       </c>
       <c r="C222" t="s">
         <v>873</v>
@@ -7561,7 +7615,7 @@
         <v>968</v>
       </c>
       <c r="B223" t="s">
-        <v>968</v>
+        <v>1074</v>
       </c>
       <c r="C223" t="s">
         <v>854</v>
@@ -7575,7 +7629,7 @@
         <v>967</v>
       </c>
       <c r="B224" t="s">
-        <v>978</v>
+        <v>1075</v>
       </c>
       <c r="C224" t="s">
         <v>857</v>
@@ -7589,7 +7643,7 @@
         <v>969</v>
       </c>
       <c r="B225" s="3" t="s">
-        <v>979</v>
+        <v>1076</v>
       </c>
       <c r="C225" s="3" t="s">
         <v>865</v>
@@ -7604,10 +7658,10 @@
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="B226" t="s">
-        <v>983</v>
+        <v>1077</v>
       </c>
       <c r="C226" t="s">
         <v>880</v>
@@ -7618,10 +7672,10 @@
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>981</v>
+        <v>978</v>
       </c>
       <c r="B227" t="s">
-        <v>981</v>
+        <v>1078</v>
       </c>
       <c r="C227" t="s">
         <v>877</v>
@@ -7632,10 +7686,10 @@
     </row>
     <row r="228" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>982</v>
+        <v>979</v>
       </c>
       <c r="B228" t="s">
-        <v>982</v>
+        <v>1079</v>
       </c>
       <c r="C228" t="s">
         <v>879</v>
@@ -7650,10 +7704,10 @@
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>988</v>
+        <v>981</v>
       </c>
       <c r="B229" t="s">
-        <v>988</v>
+        <v>1080</v>
       </c>
       <c r="D229" t="s">
         <v>693</v>
@@ -7664,7 +7718,7 @@
         <v>976</v>
       </c>
       <c r="B230" t="s">
-        <v>976</v>
+        <v>1081</v>
       </c>
       <c r="C230" t="s">
         <v>871</v>
@@ -7717,7 +7771,7 @@
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>1033</v>
+        <v>1006</v>
       </c>
       <c r="B234" t="s">
         <v>754</v>
@@ -7787,7 +7841,7 @@
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>1021</v>
+        <v>994</v>
       </c>
       <c r="B239" t="s">
         <v>733</v>
@@ -7804,7 +7858,7 @@
         <v>971</v>
       </c>
       <c r="B240" t="s">
-        <v>971</v>
+        <v>1089</v>
       </c>
       <c r="C240" t="s">
         <v>855</v>
@@ -7818,7 +7872,7 @@
         <v>970</v>
       </c>
       <c r="B241" t="s">
-        <v>991</v>
+        <v>1090</v>
       </c>
       <c r="C241" t="s">
         <v>858</v>
@@ -7832,7 +7886,7 @@
         <v>972</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>992</v>
+        <v>1091</v>
       </c>
       <c r="C242" s="3" t="s">
         <v>866</v>
@@ -7843,10 +7897,10 @@
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>996</v>
+        <v>984</v>
       </c>
       <c r="B243" t="s">
-        <v>996</v>
+        <v>1092</v>
       </c>
       <c r="C243" t="s">
         <v>884</v>
@@ -7857,10 +7911,10 @@
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>994</v>
+        <v>982</v>
       </c>
       <c r="B244" t="s">
-        <v>994</v>
+        <v>1093</v>
       </c>
       <c r="C244" t="s">
         <v>882</v>
@@ -7871,10 +7925,10 @@
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>995</v>
+        <v>983</v>
       </c>
       <c r="B245" t="s">
-        <v>995</v>
+        <v>1094</v>
       </c>
       <c r="C245" t="s">
         <v>883</v>
@@ -7885,10 +7939,10 @@
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>1001</v>
+        <v>985</v>
       </c>
       <c r="B246" t="s">
-        <v>1001</v>
+        <v>1095</v>
       </c>
       <c r="D246" t="s">
         <v>693</v>
@@ -7899,7 +7953,7 @@
         <v>975</v>
       </c>
       <c r="B247" t="s">
-        <v>975</v>
+        <v>1096</v>
       </c>
       <c r="C247" t="s">
         <v>872</v>
@@ -7910,7 +7964,7 @@
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>1022</v>
+        <v>995</v>
       </c>
       <c r="B248" t="s">
         <v>735</v>
@@ -7980,13 +8034,13 @@
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
-        <v>1035</v>
+        <v>1008</v>
       </c>
       <c r="B253" t="s">
         <v>756</v>
       </c>
       <c r="C253" t="s">
-        <v>1036</v>
+        <v>1009</v>
       </c>
       <c r="D253" t="s">
         <v>757</v>
@@ -7994,7 +8048,7 @@
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>1037</v>
+        <v>1010</v>
       </c>
       <c r="B254" t="s">
         <v>758</v>
@@ -8008,13 +8062,13 @@
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A255" s="31" t="s">
-        <v>1050</v>
+        <v>1023</v>
       </c>
       <c r="B255" t="s">
         <v>817</v>
       </c>
       <c r="C255" t="s">
-        <v>1049</v>
+        <v>1022</v>
       </c>
       <c r="D255" t="s">
         <v>797</v>
@@ -8022,7 +8076,7 @@
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>1038</v>
+        <v>1011</v>
       </c>
       <c r="B256" t="s">
         <v>760</v>
@@ -8078,7 +8132,7 @@
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
-        <v>1034</v>
+        <v>1007</v>
       </c>
       <c r="B260" t="s">
         <v>63</v>
@@ -8106,7 +8160,7 @@
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A262" s="31" t="s">
-        <v>1040</v>
+        <v>1013</v>
       </c>
       <c r="B262" t="s">
         <v>751</v>
@@ -8120,7 +8174,7 @@
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A263" s="31" t="s">
-        <v>1041</v>
+        <v>1014</v>
       </c>
       <c r="B263" t="s">
         <v>750</v>
@@ -8134,7 +8188,7 @@
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A264" s="31" t="s">
-        <v>1039</v>
+        <v>1012</v>
       </c>
       <c r="B264" t="s">
         <v>749</v>
@@ -8148,7 +8202,7 @@
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A265" s="3" t="s">
-        <v>1026</v>
+        <v>999</v>
       </c>
       <c r="B265" t="s">
         <v>746</v>
@@ -8162,7 +8216,7 @@
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A266" s="3" t="s">
-        <v>1023</v>
+        <v>996</v>
       </c>
       <c r="B266" t="s">
         <v>742</v>
@@ -8176,13 +8230,13 @@
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
-        <v>1029</v>
+        <v>1002</v>
       </c>
       <c r="B267" t="s">
         <v>791</v>
       </c>
       <c r="C267" t="s">
-        <v>1043</v>
+        <v>1016</v>
       </c>
       <c r="D267" t="s">
         <v>693</v>
@@ -8190,7 +8244,7 @@
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A268" s="3" t="s">
-        <v>1027</v>
+        <v>1000</v>
       </c>
       <c r="B268" t="s">
         <v>747</v>
@@ -8204,7 +8258,7 @@
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A269" s="3" t="s">
-        <v>1024</v>
+        <v>997</v>
       </c>
       <c r="B269" t="s">
         <v>744</v>
@@ -8218,13 +8272,13 @@
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
-        <v>1030</v>
+        <v>1003</v>
       </c>
       <c r="B270" t="s">
         <v>792</v>
       </c>
       <c r="C270" t="s">
-        <v>1042</v>
+        <v>1015</v>
       </c>
       <c r="D270" t="s">
         <v>693</v>
@@ -8232,7 +8286,7 @@
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A271" s="3" t="s">
-        <v>1028</v>
+        <v>1001</v>
       </c>
       <c r="B271" t="s">
         <v>748</v>
@@ -8246,7 +8300,7 @@
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A272" s="3" t="s">
-        <v>1025</v>
+        <v>998</v>
       </c>
       <c r="B272" t="s">
         <v>745</v>
@@ -8260,13 +8314,13 @@
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
-        <v>1031</v>
+        <v>1004</v>
       </c>
       <c r="B273" t="s">
         <v>793</v>
       </c>
       <c r="C273" t="s">
-        <v>1044</v>
+        <v>1017</v>
       </c>
       <c r="D273" t="s">
         <v>693</v>
@@ -8400,7 +8454,7 @@
         <v>226</v>
       </c>
       <c r="B283" t="s">
-        <v>980</v>
+        <v>1082</v>
       </c>
       <c r="C283" t="s">
         <v>874</v>
@@ -8414,7 +8468,7 @@
         <v>226</v>
       </c>
       <c r="B284" t="s">
-        <v>993</v>
+        <v>1097</v>
       </c>
       <c r="C284" t="s">
         <v>875</v>
@@ -8428,7 +8482,7 @@
         <v>226</v>
       </c>
       <c r="B285" t="s">
-        <v>1006</v>
+        <v>1067</v>
       </c>
       <c r="C285" t="s">
         <v>876</v>
@@ -8456,7 +8510,7 @@
         <v>226</v>
       </c>
       <c r="B287" t="s">
-        <v>984</v>
+        <v>1083</v>
       </c>
       <c r="C287" t="s">
         <v>881</v>
@@ -8470,7 +8524,7 @@
         <v>226</v>
       </c>
       <c r="B288" t="s">
-        <v>985</v>
+        <v>1084</v>
       </c>
       <c r="C288" t="s">
         <v>878</v>
@@ -8484,7 +8538,7 @@
         <v>226</v>
       </c>
       <c r="B289" t="s">
-        <v>997</v>
+        <v>1098</v>
       </c>
       <c r="C289" t="s">
         <v>885</v>
@@ -8498,7 +8552,7 @@
         <v>226</v>
       </c>
       <c r="B290" t="s">
-        <v>998</v>
+        <v>1099</v>
       </c>
       <c r="C290" t="s">
         <v>878</v>
@@ -8512,7 +8566,7 @@
         <v>226</v>
       </c>
       <c r="B291" t="s">
-        <v>1010</v>
+        <v>1068</v>
       </c>
       <c r="C291" t="s">
         <v>889</v>
@@ -8526,7 +8580,7 @@
         <v>226</v>
       </c>
       <c r="B292" t="s">
-        <v>1011</v>
+        <v>1069</v>
       </c>
       <c r="C292" t="s">
         <v>878</v>
@@ -8862,7 +8916,7 @@
         <v>226</v>
       </c>
       <c r="B316" t="s">
-        <v>986</v>
+        <v>1085</v>
       </c>
       <c r="C316" t="s">
         <v>933</v>
@@ -8876,7 +8930,7 @@
         <v>226</v>
       </c>
       <c r="B317" t="s">
-        <v>987</v>
+        <v>1086</v>
       </c>
       <c r="C317" t="s">
         <v>934</v>
@@ -8890,7 +8944,7 @@
         <v>226</v>
       </c>
       <c r="B318" t="s">
-        <v>999</v>
+        <v>1100</v>
       </c>
       <c r="C318" t="s">
         <v>933</v>
@@ -8904,7 +8958,7 @@
         <v>226</v>
       </c>
       <c r="B319" t="s">
-        <v>1000</v>
+        <v>1101</v>
       </c>
       <c r="C319" t="s">
         <v>934</v>
@@ -8918,7 +8972,7 @@
         <v>226</v>
       </c>
       <c r="B320" t="s">
-        <v>1012</v>
+        <v>1070</v>
       </c>
       <c r="C320" t="s">
         <v>933</v>
@@ -8932,7 +8986,7 @@
         <v>226</v>
       </c>
       <c r="B321" t="s">
-        <v>1013</v>
+        <v>1071</v>
       </c>
       <c r="C321" t="s">
         <v>934</v>
@@ -8978,7 +9032,7 @@
       </c>
       <c r="C324" s="3"/>
       <c r="D324" t="s">
-        <v>1014</v>
+        <v>989</v>
       </c>
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.3">
@@ -8990,7 +9044,7 @@
       </c>
       <c r="C325" s="3"/>
       <c r="D325" t="s">
-        <v>1014</v>
+        <v>989</v>
       </c>
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.3">
@@ -9002,7 +9056,7 @@
       </c>
       <c r="C326" s="3"/>
       <c r="D326" t="s">
-        <v>1014</v>
+        <v>989</v>
       </c>
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.3">
@@ -9014,7 +9068,7 @@
       </c>
       <c r="C327" s="3"/>
       <c r="D327" t="s">
-        <v>1014</v>
+        <v>989</v>
       </c>
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.3">
@@ -9026,7 +9080,7 @@
       </c>
       <c r="C328" s="3"/>
       <c r="D328" t="s">
-        <v>1014</v>
+        <v>989</v>
       </c>
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.3">
@@ -9038,7 +9092,7 @@
       </c>
       <c r="C329" s="3"/>
       <c r="D329" t="s">
-        <v>1014</v>
+        <v>989</v>
       </c>
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.3">
@@ -9050,7 +9104,7 @@
       </c>
       <c r="C330" s="3"/>
       <c r="D330" t="s">
-        <v>1014</v>
+        <v>989</v>
       </c>
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.3">
@@ -9062,7 +9116,7 @@
       </c>
       <c r="C331" s="3"/>
       <c r="D331" t="s">
-        <v>1014</v>
+        <v>989</v>
       </c>
     </row>
     <row r="332" spans="1:4" x14ac:dyDescent="0.3">
@@ -9074,7 +9128,7 @@
       </c>
       <c r="C332" s="3"/>
       <c r="D332" t="s">
-        <v>1015</v>
+        <v>990</v>
       </c>
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.3">
@@ -9086,7 +9140,7 @@
       </c>
       <c r="C333" s="3"/>
       <c r="D333" t="s">
-        <v>1015</v>
+        <v>990</v>
       </c>
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.3">
@@ -9504,7 +9558,7 @@
         <v>226</v>
       </c>
       <c r="B371" t="s">
-        <v>989</v>
+        <v>1087</v>
       </c>
       <c r="D371" t="s">
         <v>833</v>
@@ -9515,7 +9569,7 @@
         <v>226</v>
       </c>
       <c r="B372" t="s">
-        <v>1002</v>
+        <v>1102</v>
       </c>
       <c r="D372" t="s">
         <v>833</v>
@@ -9526,7 +9580,7 @@
         <v>226</v>
       </c>
       <c r="B373" t="s">
-        <v>1017</v>
+        <v>1072</v>
       </c>
       <c r="D373" t="s">
         <v>833</v>
@@ -9559,7 +9613,7 @@
         <v>226</v>
       </c>
       <c r="B376" t="s">
-        <v>990</v>
+        <v>1088</v>
       </c>
       <c r="D376" t="s">
         <v>833</v>
@@ -9570,7 +9624,7 @@
         <v>226</v>
       </c>
       <c r="B377" t="s">
-        <v>1003</v>
+        <v>1103</v>
       </c>
       <c r="D377" t="s">
         <v>833</v>
@@ -9581,7 +9635,7 @@
         <v>226</v>
       </c>
       <c r="B378" t="s">
-        <v>1018</v>
+        <v>1073</v>
       </c>
       <c r="D378" t="s">
         <v>833</v>
@@ -45674,7 +45728,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -45709,7 +45763,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
-        <v>1051</v>
+        <v>1024</v>
       </c>
       <c r="E4" s="18"/>
     </row>
@@ -45721,25 +45775,25 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B6" s="21" t="s">
-        <v>1082</v>
+        <v>1055</v>
       </c>
       <c r="E6" s="18"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B7" s="21" t="s">
-        <v>1083</v>
+        <v>1056</v>
       </c>
       <c r="E7" s="18"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8" s="21" t="s">
-        <v>1084</v>
+        <v>1057</v>
       </c>
       <c r="E8" s="18"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B9" s="21" t="s">
-        <v>1085</v>
+        <v>1058</v>
       </c>
       <c r="E9" s="18"/>
     </row>
@@ -45787,7 +45841,7 @@
         <v>203</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>1072</v>
+        <v>1045</v>
       </c>
       <c r="F13" t="s">
         <v>376</v>
@@ -45818,7 +45872,7 @@
         <v>945</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>1054</v>
+        <v>1027</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>554</v>
@@ -45838,7 +45892,7 @@
         <v>454</v>
       </c>
       <c r="B16" t="s">
-        <v>1057</v>
+        <v>1030</v>
       </c>
       <c r="C16" t="s">
         <v>208</v>
@@ -45858,7 +45912,7 @@
         <v>456</v>
       </c>
       <c r="B17" t="s">
-        <v>1058</v>
+        <v>1031</v>
       </c>
       <c r="C17" t="s">
         <v>208</v>
@@ -45878,7 +45932,7 @@
         <v>455</v>
       </c>
       <c r="B18" t="s">
-        <v>1059</v>
+        <v>1032</v>
       </c>
       <c r="C18" t="s">
         <v>208</v>
@@ -45898,7 +45952,7 @@
         <v>408</v>
       </c>
       <c r="B19" t="s">
-        <v>1052</v>
+        <v>1025</v>
       </c>
       <c r="C19" t="s">
         <v>394</v>
@@ -45907,7 +45961,7 @@
         <v>117</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>1072</v>
+        <v>1045</v>
       </c>
       <c r="F19" t="s">
         <v>376</v>
@@ -45918,7 +45972,7 @@
         <v>408</v>
       </c>
       <c r="B20" t="s">
-        <v>1068</v>
+        <v>1041</v>
       </c>
       <c r="C20" t="s">
         <v>394</v>
@@ -45927,7 +45981,7 @@
         <v>117</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>1072</v>
+        <v>1045</v>
       </c>
       <c r="F20" t="s">
         <v>376</v>
@@ -45935,10 +45989,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>1075</v>
+        <v>1048</v>
       </c>
       <c r="B21" t="s">
-        <v>1067</v>
+        <v>1040</v>
       </c>
       <c r="C21" t="s">
         <v>512</v>
@@ -45947,7 +46001,7 @@
         <v>364</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>1076</v>
+        <v>1049</v>
       </c>
       <c r="F21" t="s">
         <v>511</v>
@@ -46058,7 +46112,7 @@
         <v>955</v>
       </c>
       <c r="B27" t="s">
-        <v>1062</v>
+        <v>1035</v>
       </c>
       <c r="C27" t="s">
         <v>550</v>
@@ -46078,7 +46132,7 @@
         <v>956</v>
       </c>
       <c r="B28" t="s">
-        <v>1060</v>
+        <v>1033</v>
       </c>
       <c r="C28" t="s">
         <v>552</v>
@@ -46098,7 +46152,7 @@
         <v>956</v>
       </c>
       <c r="B29" t="s">
-        <v>1061</v>
+        <v>1034</v>
       </c>
       <c r="C29" t="s">
         <v>552</v>
@@ -46115,10 +46169,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>1077</v>
+        <v>1050</v>
       </c>
       <c r="B30" t="s">
-        <v>1064</v>
+        <v>1037</v>
       </c>
       <c r="C30" t="s">
         <v>678</v>
@@ -46127,50 +46181,50 @@
         <v>142</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>1080</v>
+        <v>1053</v>
       </c>
       <c r="F30" t="s">
-        <v>1081</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>1078</v>
+        <v>1051</v>
       </c>
       <c r="B31" t="s">
-        <v>1065</v>
+        <v>1038</v>
       </c>
       <c r="C31" t="s">
-        <v>1073</v>
+        <v>1046</v>
       </c>
       <c r="D31" t="s">
         <v>142</v>
       </c>
       <c r="E31" s="18" t="s">
-        <v>1080</v>
+        <v>1053</v>
       </c>
       <c r="F31" t="s">
-        <v>1081</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>1079</v>
+        <v>1052</v>
       </c>
       <c r="B32" t="s">
-        <v>1066</v>
+        <v>1039</v>
       </c>
       <c r="C32" t="s">
-        <v>1074</v>
+        <v>1047</v>
       </c>
       <c r="D32" t="s">
         <v>142</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>1080</v>
+        <v>1053</v>
       </c>
       <c r="F32" t="s">
-        <v>1081</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -46187,7 +46241,7 @@
         <v>203</v>
       </c>
       <c r="E33" s="18" t="s">
-        <v>1072</v>
+        <v>1045</v>
       </c>
       <c r="F33" t="s">
         <v>376</v>
@@ -46218,10 +46272,10 @@
         <v>226</v>
       </c>
       <c r="B35" t="s">
-        <v>1055</v>
+        <v>1028</v>
       </c>
       <c r="C35" t="s">
-        <v>1071</v>
+        <v>1044</v>
       </c>
       <c r="D35" t="s">
         <v>39</v>
@@ -46238,10 +46292,10 @@
         <v>226</v>
       </c>
       <c r="B36" t="s">
-        <v>1056</v>
+        <v>1029</v>
       </c>
       <c r="C36" t="s">
-        <v>1070</v>
+        <v>1043</v>
       </c>
       <c r="D36" t="s">
         <v>39</v>
@@ -46318,7 +46372,7 @@
         <v>226</v>
       </c>
       <c r="B40" t="s">
-        <v>1053</v>
+        <v>1026</v>
       </c>
       <c r="C40" t="s">
         <v>509</v>
@@ -46327,7 +46381,7 @@
         <v>142</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>1072</v>
+        <v>1045</v>
       </c>
       <c r="F40" t="s">
         <v>376</v>
@@ -46338,7 +46392,7 @@
         <v>226</v>
       </c>
       <c r="B41" t="s">
-        <v>1069</v>
+        <v>1042</v>
       </c>
       <c r="C41" t="s">
         <v>509</v>
@@ -46347,7 +46401,7 @@
         <v>142</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>1072</v>
+        <v>1045</v>
       </c>
       <c r="F41" t="s">
         <v>376</v>
@@ -46378,7 +46432,7 @@
         <v>226</v>
       </c>
       <c r="B43" t="s">
-        <v>1063</v>
+        <v>1036</v>
       </c>
       <c r="C43" t="s">
         <v>550</v>

</xml_diff>

<commit_message>
Fix wind direction issue
</commit_message>
<xml_diff>
--- a/Resources/EmpreinteVariableDescription.xlsx
+++ b/Resources/EmpreinteVariableDescription.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="819" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="819" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Berge_cs" sheetId="1" r:id="rId1"/>
@@ -7471,8 +7471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -52872,7 +52872,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A24" workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
@@ -54976,8 +54976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L156"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>